<commit_message>
Endplate completed. Hopefully it won't break immediately.
</commit_message>
<xml_diff>
--- a/Endplate/Endplate__new.xlsx
+++ b/Endplate/Endplate__new.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="45" yWindow="0" windowWidth="9165" windowHeight="7590"/>
+    <workbookView visibility="veryHidden" xWindow="45" yWindow="0" windowWidth="9810" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MainPlate" sheetId="2" r:id="rId2"/>
+    <sheet name="SecondaryPlate" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Family">Sheet1!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Design Table for: Endplate</t>
   </si>
@@ -49,22 +51,28 @@
     <t>D1@SecondaryPlate</t>
   </si>
   <si>
-    <t>D1@Sketch21</t>
-  </si>
-  <si>
-    <t>D1@Sketch22</t>
-  </si>
-  <si>
-    <t>D1@Sketch25</t>
-  </si>
-  <si>
-    <t>D1@Sketch27</t>
-  </si>
-  <si>
-    <t>D1@Sketch26</t>
-  </si>
-  <si>
-    <t>D1@Sketch28</t>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>FirstAngleofDivergence</t>
+  </si>
+  <si>
+    <t>SecondAngleofDivergence</t>
+  </si>
+  <si>
+    <t>LineOfDivergence</t>
+  </si>
+  <si>
+    <t>AngleOfDivergence</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
@@ -117,7 +125,23 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,6 +149,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Configuration"/>
+    <tableColumn id="2" name="FirstAngleofDivergence"/>
+    <tableColumn id="3" name="SecondAngleofDivergence"/>
+    <tableColumn id="4" name="Height" dataDxfId="4"/>
+    <tableColumn id="5" name="Width" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Configuration"/>
+    <tableColumn id="2" name="LineOfDivergence" dataDxfId="2"/>
+    <tableColumn id="3" name="AngleOfDivergence" dataDxfId="1"/>
+    <tableColumn id="4" name="Length" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,15 +476,14 @@
     <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="3.7109375" style="2" customWidth="1"/>
     <col min="4" max="8" width="12.85546875" style="2" customWidth="1"/>
-    <col min="9" max="14" width="3.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="154.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="5" customFormat="1" ht="154.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -456,90 +506,177 @@
       <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
+        <f>MainPlate!B2</f>
         <v>3</v>
       </c>
       <c r="C3" s="2">
+        <f>MainPlate!C2</f>
         <v>3</v>
       </c>
       <c r="D3" s="2">
+        <f>MainPlate!D2</f>
         <v>7.5175668582005528E-2</v>
       </c>
       <c r="E3" s="2">
+        <f>MainPlate!E2</f>
         <v>7.8244683948184957E-2</v>
       </c>
       <c r="F3" s="2">
+        <f>SecondaryPlate!B2</f>
         <v>13.165436579062279</v>
       </c>
       <c r="G3" s="2">
+        <f>SecondaryPlate!C2</f>
         <v>24.343323050707831</v>
       </c>
       <c r="H3" s="2">
+        <f>SecondaryPlate!D2</f>
         <v>0.19627477562809914</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Plane2" prompt="Enter a valid value for this parameter." sqref="B3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@MainPlane" prompt="Enter a valid value for this parameter." sqref="C3"/>
+  <dataValidations count="6">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Plane2" prompt="Enter a valid value for this parameter." sqref="B3:C3"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@EndplateMainDimensions" prompt="Enter a valid value for this parameter." sqref="D3"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D2@EndplateMainDimensions" prompt="Enter a valid value for this parameter." sqref="E3"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@LineOfDivergence" prompt="Enter a valid value for this parameter." sqref="F3"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@PlaneAxis3" prompt="Enter a valid value for this parameter." sqref="G3"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@SecondaryPlate" prompt="Enter a valid value for this parameter." sqref="H3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch21" prompt="Enter a valid value for this parameter." sqref="I3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch22" prompt="Enter a valid value for this parameter." sqref="J3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch25" prompt="Enter a valid value for this parameter." sqref="K3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch27" prompt="Enter a valid value for this parameter." sqref="L3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch26" prompt="Enter a valid value for this parameter." sqref="M3"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@Sketch28" prompt="Enter a valid value for this parameter." sqref="N3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>7.5175668582005528E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7.8244683948184957E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@EndplateMainDimensions" prompt="Enter a valid value for this parameter." sqref="D2:D3"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D2@EndplateMainDimensions" prompt="Enter a valid value for this parameter." sqref="E2:E3"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>13.165436579062279</v>
+      </c>
+      <c r="C2" s="2">
+        <v>24.343323050707831</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.19627477562809914</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@LineOfDivergence" prompt="Enter a valid value for this parameter." sqref="B2"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@PlaneAxis3" prompt="Enter a valid value for this parameter." sqref="C2"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="SOLIDWORKS Error:" error="The value you have entered is invalid.  Please enter a valid value before continuing." promptTitle="D1@SecondaryPlate" prompt="Enter a valid value for this parameter." sqref="D2"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>